<commit_message>
updated couns process, w view and edit evaulation
with test db
</commit_message>
<xml_diff>
--- a/sample file for importing excel file/student.xlsx
+++ b/sample file for importing excel file/student.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ermil Magtuloy\Documents\GitHub\PUPBC-Student-Counceling-and-Violation-System\sample file for importing excel file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PUPBC Counseling and Violation System\sample file for importing excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000B4BF-252D-406D-AEF6-ED671F4DAB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDEF060-EA9C-4221-A651-09DBAF0E6D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>BSIT</t>
   </si>
@@ -69,7 +69,10 @@
     <t xml:space="preserve">Sample with Barangay City Municipality and Country </t>
   </si>
   <si>
-    <t>AYCODE</t>
+    <t>2022, 2023 - 2nd</t>
+  </si>
+  <si>
+    <t>BATCHYEAR</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,6 +404,7 @@
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -429,7 +433,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -456,6 +460,9 @@
       </c>
       <c r="H2" t="s">
         <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated 02 25 2022
</commit_message>
<xml_diff>
--- a/sample file for importing excel file/student.xlsx
+++ b/sample file for importing excel file/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PUPBC Counseling and Violation System\sample file for importing excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDEF060-EA9C-4221-A651-09DBAF0E6D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FBB948-844A-456E-B49C-01B189E61E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>BSIT</t>
   </si>
@@ -73,16 +73,58 @@
   </si>
   <si>
     <t>BATCHYEAR</t>
+  </si>
+  <si>
+    <t>Sadasdasda</t>
+  </si>
+  <si>
+    <t>Sample Chazxczxczxnge</t>
+  </si>
+  <si>
+    <t>Samplezczxcz</t>
+  </si>
+  <si>
+    <t>Sampleadad</t>
+  </si>
+  <si>
+    <t>qeqqweqw</t>
+  </si>
+  <si>
+    <t>Samplejkjkhj</t>
+  </si>
+  <si>
+    <t>Samplesfsdf</t>
+  </si>
+  <si>
+    <t>Samplesfsfd</t>
+  </si>
+  <si>
+    <t>Samplekjkkuku</t>
+  </si>
+  <si>
+    <t>2018-11111-BN-0</t>
+  </si>
+  <si>
+    <t>2018-03300-BN-2</t>
+  </si>
+  <si>
+    <t>2018-00550-BN-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,17 +432,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I2" sqref="I2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
@@ -447,7 +489,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -465,7 +507,95 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated validation, with reponsive reg ui with db
</commit_message>
<xml_diff>
--- a/sample file for importing excel file/student.xlsx
+++ b/sample file for importing excel file/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PUPBC Counseling and Violation System\sample file for importing excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FBB948-844A-456E-B49C-01B189E61E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6037D1EF-48F8-4BC4-9E18-C9A5CA2CD025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>PROGRAM</t>
   </si>
   <si>
-    <t>2018-00000-BN-0</t>
-  </si>
-  <si>
     <t>Sample</t>
   </si>
   <si>
@@ -102,13 +99,16 @@
     <t>Samplekjkkuku</t>
   </si>
   <si>
-    <t>2018-11111-BN-0</t>
-  </si>
-  <si>
-    <t>2018-03300-BN-2</t>
-  </si>
-  <si>
-    <t>2018-00550-BN-3</t>
+    <t>2018-00069-BN-0</t>
+  </si>
+  <si>
+    <t>2018-11170-BN-0</t>
+  </si>
+  <si>
+    <t>2018-03371-BN-2</t>
+  </si>
+  <si>
+    <t>2018-00572-BN-3</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,16 +451,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -475,36 +475,36 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -512,28 +512,28 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -541,28 +541,28 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -570,28 +570,28 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with unactive role and user account
</commit_message>
<xml_diff>
--- a/sample file for importing excel file/student.xlsx
+++ b/sample file for importing excel file/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PUPBC Counseling and Violation System\sample file for importing excel file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6037D1EF-48F8-4BC4-9E18-C9A5CA2CD025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E43F89-ED6D-474B-8450-C716B8586C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>BSIT</t>
   </si>
@@ -42,9 +42,6 @@
     <t>PROGRAM</t>
   </si>
   <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Sample Chazxczxczxnge</t>
   </si>
   <si>
-    <t>Samplezczxcz</t>
-  </si>
-  <si>
     <t>Sampleadad</t>
   </si>
   <si>
@@ -109,6 +103,15 @@
   </si>
   <si>
     <t>2018-00572-BN-3</t>
+  </si>
+  <si>
+    <t>Benito</t>
+  </si>
+  <si>
+    <t>Cortes</t>
+  </si>
+  <si>
+    <t>Masubong</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,16 +454,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -475,123 +478,123 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>